<commit_message>
Added Berkeley and UChicago faculty interests
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\transit_credit-access\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90BFBD-15EB-4580-A25E-7B6E8636E2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BD36F2-0378-9045-9AA3-C7C086407ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27375" yWindow="3090" windowWidth="21795" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>School</t>
   </si>
@@ -171,23 +171,78 @@
     <t>Emory</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deadline </t>
   </si>
   <si>
-    <t xml:space="preserve">Application opens </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open now </t>
+    <t xml:space="preserve">Faculty to mention </t>
+  </si>
+  <si>
+    <t>Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resume? </t>
+  </si>
+  <si>
+    <t>Writing sample length</t>
+  </si>
+  <si>
+    <t># letters of rec</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Other requirements?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800 word research statement </t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Gottlieb -- place-based policies. Jeffrey Grogger -- inequality and applied micro. Kelly Hallburg -- segregation, disinvestment. Damon Jones -- racial differences in financial outcomes. Paula Worthington -- metropolitan investment and super applied. </t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional </t>
+  </si>
+  <si>
+    <t>SoP Notes</t>
+  </si>
+  <si>
+    <t>300 word motivation statement</t>
+  </si>
+  <si>
+    <t>Additional optional essays</t>
+  </si>
+  <si>
+    <t>3 pages double spaced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal history statement (same length as SoP). Must explicitly mention 2 faculty members to work with. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total applications cost: </t>
+  </si>
+  <si>
+    <t>Cecile Gaubert -- high-speed rail and spatial sorting &amp; inequality. Hilary Hoynes -- inequality. Pat Kline -- trends in spatial inequality.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -213,6 +268,26 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,18 +306,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -460,22 +546,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,74 +574,170 @@
       <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="6">
+        <v>45266</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7">
+        <v>200</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="6">
+        <v>45204</v>
+      </c>
+      <c r="D3" t="str">
+        <f>D2</f>
+        <v xml:space="preserve">Joshua Gottlieb -- place-based policies. Jeffrey Grogger -- inequality and applied micro. Kelly Hallburg -- segregation, disinvestment. Damon Jones -- racial differences in financial outcomes. Paula Worthington -- metropolitan investment and super applied. </v>
+      </c>
+      <c r="E3" s="9">
+        <v>100</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="6">
+        <v>45204</v>
+      </c>
+      <c r="D4" t="str">
+        <f>D2</f>
+        <v xml:space="preserve">Joshua Gottlieb -- place-based policies. Jeffrey Grogger -- inequality and applied micro. Kelly Hallburg -- segregation, disinvestment. Damon Jones -- racial differences in financial outcomes. Paula Worthington -- metropolitan investment and super applied. </v>
+      </c>
+      <c r="E4" s="9">
+        <v>100</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3">
-        <v>45184</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="3">
         <v>45264</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="9">
+        <v>135</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="3">
+      <c r="C6" s="3">
         <v>45278</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -560,7 +745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -568,21 +753,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="C9" s="3">
         <v>45261</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -590,7 +772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -598,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -606,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -614,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -622,22 +804,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -645,7 +827,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -653,7 +835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -661,17 +843,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="43" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="11">
+        <f>SUM(E:E)</f>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -704,18 +895,18 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -772,7 +963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -783,7 +974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -791,7 +982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -799,7 +990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -807,7 +998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -815,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -823,7 +1014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -831,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -842,7 +1033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -850,7 +1041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -858,7 +1049,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -869,7 +1060,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -877,7 +1068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -885,7 +1076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -893,7 +1084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -901,7 +1092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -909,7 +1100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -917,22 +1108,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -940,7 +1131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -948,7 +1139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -956,12 +1147,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Added comments for Wharton
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F4E86-6ACC-2F47-800B-1A0EDFCC339B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9CAF14-9E91-6B4A-A019-4BA418963DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>School</t>
   </si>
@@ -317,7 +317,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,6 +332,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -773,6 +774,27 @@
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="12">
+        <v>45275</v>
+      </c>
+      <c r="E8" s="9">
+        <v>80</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
@@ -883,7 +905,7 @@
       </c>
       <c r="B25" s="11">
         <f>SUM(E:E)</f>
-        <v>645</v>
+        <v>725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More or less wrapped up first draft
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\arc\dfs\unix\scratch\m1kms01\transit_credit-access\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0D8495-5393-1D49-AD1E-EDD34D1D8234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A11A14-95BA-4354-A371-57774E5FF378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -684,22 +684,22 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" customWidth="1"/>
+    <col min="3" max="3" width="11.15234375" customWidth="1"/>
+    <col min="4" max="4" width="19.4609375" customWidth="1"/>
+    <col min="5" max="5" width="6.4609375" customWidth="1"/>
+    <col min="6" max="6" width="8.69140625" customWidth="1"/>
+    <col min="7" max="7" width="14.15234375" customWidth="1"/>
+    <col min="8" max="8" width="18.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -793,7 +793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -825,7 +825,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -886,7 +886,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -918,7 +918,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -950,7 +950,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -982,7 +982,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>83</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>89</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>88</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1320,10 +1320,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <f>MIN(C2:C20)</f>
+        <v>44930</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>63</v>
       </c>
@@ -1333,7 +1336,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
     </row>
   </sheetData>
@@ -1374,15 +1377,15 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" customWidth="1"/>
+    <col min="3" max="3" width="11.15234375" customWidth="1"/>
+    <col min="4" max="5" width="19.4609375" customWidth="1"/>
+    <col min="6" max="6" width="16.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1584,22 +1587,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1623,12 +1626,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Swapped UVA for UNC, added Yale
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\arc\dfs\unix\scratch\m1kms01\transit_credit-access\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A11A14-95BA-4354-A371-57774E5FF378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3836AF43-8C00-4A22-86F1-F8D7730681D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
   <si>
     <t>School</t>
   </si>
@@ -342,9 +342,6 @@
     <t xml:space="preserve">Rachel Kranton -- network effects.Patrick Bayer -- racial discrimination.  Jason Baron -- really cool foster care work. Overall awesome faculty, a lot of potential advisors and cool people </t>
   </si>
   <si>
-    <t>Luca Flabbi -- gender dynamics in the labor market. Jane Fruehwirth -- education and desegregation effects. Chris Handy -- intergenerational mobility.</t>
-  </si>
-  <si>
     <t>2 pages single spaced</t>
   </si>
   <si>
@@ -361,6 +358,30 @@
   </si>
   <si>
     <t>Will Dobbie -- housing discrimination. Luis Armona -- home price expectations. Desmond Ang -- violence on inner-city students.</t>
+  </si>
+  <si>
+    <t>Joseph Altonji -- cool research on the role of families and schools in inequality. Gerald Jaynes -- research on Black participation in the labor market and effects of migration on the Black working class (possibly emeritus?). Ed Vytlacil -- evaluating disparate returns to schooling, speaks to disparate impact of treatment effects (like my NSF proposal).</t>
+  </si>
+  <si>
+    <t>500-1000 words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsure? </t>
+  </si>
+  <si>
+    <t>Econ Ranking</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>UVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Pepper -- cool policy evaluation work. Sarah Turner -- disparate returns to higher education, inequality. Amalia Miller -- gender labor papers. </t>
   </si>
 </sst>
 </file>
@@ -681,229 +702,248 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.4609375" customWidth="1"/>
-    <col min="3" max="3" width="11.15234375" customWidth="1"/>
-    <col min="4" max="4" width="19.4609375" customWidth="1"/>
-    <col min="5" max="5" width="6.4609375" customWidth="1"/>
-    <col min="6" max="6" width="8.69140625" customWidth="1"/>
-    <col min="7" max="7" width="14.15234375" customWidth="1"/>
-    <col min="8" max="8" width="18.4609375" customWidth="1"/>
+    <col min="3" max="3" width="14.4609375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.15234375" customWidth="1"/>
+    <col min="5" max="5" width="19.4609375" customWidth="1"/>
+    <col min="6" max="6" width="6.4609375" customWidth="1"/>
+    <col min="7" max="7" width="8.69140625" customWidth="1"/>
+    <col min="8" max="8" width="14.15234375" customWidth="1"/>
+    <col min="9" max="9" width="18.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="5">
         <v>45266</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>200</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="5">
         <v>45204</v>
       </c>
-      <c r="D3" t="str">
-        <f>D2</f>
+      <c r="E3" t="str">
+        <f>E2</f>
         <v xml:space="preserve">Joshua Gottlieb -- place-based policies. Jeffrey Grogger -- inequality and applied micro. Kelly Hallburg -- segregation, disinvestment. Damon Jones -- racial differences in financial outcomes. Paula Worthington -- metropolitan investment and super applied. </v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
         <v>45264</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="8">
         <v>135</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
         <v>45278</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="8">
+      <c r="F5" s="8">
         <v>110</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3">
         <v>45306</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="8">
+      <c r="F6" s="8">
         <v>80</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="3">
         <v>45275</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F7" s="8">
         <v>80</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>55</v>
@@ -911,433 +951,513 @@
       <c r="H7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>45261</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F8" s="8">
         <v>90</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3">
         <v>45292</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="8">
+      <c r="F9" s="8">
         <v>75</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3">
         <v>45261</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="8">
+      <c r="F10" s="8">
         <v>75</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
         <v>45274</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="8">
+      <c r="F11" s="8">
         <v>120</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
         <v>45261</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="8">
+      <c r="F12" s="8">
         <v>75</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>3</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="14">
+      <c r="F13" s="14">
         <v>100</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>2</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="K13" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>45265</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3">
         <v>44930</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F16" s="8">
         <v>90</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3">
-        <v>45272</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="8">
-        <v>95</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="C17" s="4">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45306</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="8">
+        <v>85</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
         <v>45275</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="8">
         <v>75</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="H18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>3</v>
       </c>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="8">
+      <c r="F19" s="8">
         <v>100</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="H19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="3">
         <v>45261</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="8">
+        <v>100</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45261</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="8">
-        <v>100</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20">
+      <c r="F21" s="8">
+        <v>105</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="3">
-        <f>MIN(C2:C20)</f>
-        <v>44930</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="10">
-        <f>SUM(E:E)</f>
-        <v>1600</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
+        <f>SUM(F:F)</f>
+        <v>1695</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f>_xlfn.QUARTILE.INC(C:C,1)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <f>_xlfn.QUARTILE.INC(C:C,2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f>_xlfn.QUARTILE.INC(C:C,3)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f>_xlfn.QUARTILE.INC(C:C,4)</f>
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1358,11 +1478,12 @@
     <hyperlink ref="B14" r:id="rId15" xr:uid="{7C6CE824-AE30-494D-B258-0054A0D899EA}"/>
     <hyperlink ref="B15" r:id="rId16" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
     <hyperlink ref="B16" r:id="rId17" xr:uid="{1B93CA37-878D-49EE-B5EB-04AB17E9D9F3}"/>
-    <hyperlink ref="B17" r:id="rId18" xr:uid="{B0D76AAF-EEBA-B84E-9E94-1054BCB2B39F}"/>
-    <hyperlink ref="B18" r:id="rId19" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
+    <hyperlink ref="B17" r:id="rId20" xr:uid="{27EAEAD3-5A22-45D5-8B9B-93351924D911}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri"&amp;11&amp;K000000PERSONAL/NONWORK // EXTERNAL&amp;1#</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
More or less final list
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\arc\dfs\unix\scratch\m1kms01\transit_credit-access\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\transit_credit-access\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD09601-125F-43AE-AE07-B21A9F071945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FE07B1-68EC-44FA-860B-3D5FF331AAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-45" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="114">
   <si>
     <t>School</t>
   </si>
@@ -376,12 +376,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>UVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Pepper -- cool policy evaluation work. Sarah Turner -- disparate returns to higher education, inequality. Amalia Miller -- gender labor papers. </t>
   </si>
 </sst>
 </file>
@@ -462,7 +456,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,7 +475,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -702,26 +695,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.4609375" customWidth="1"/>
-    <col min="3" max="3" width="14.4609375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.15234375" customWidth="1"/>
-    <col min="5" max="5" width="19.4609375" customWidth="1"/>
-    <col min="6" max="6" width="6.4609375" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" customWidth="1"/>
-    <col min="8" max="8" width="14.15234375" customWidth="1"/>
-    <col min="9" max="9" width="18.4609375" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" customWidth="1"/>
+    <col min="3" max="3" width="14.46484375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" customWidth="1"/>
+    <col min="5" max="5" width="19.46484375" customWidth="1"/>
+    <col min="6" max="6" width="6.46484375" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +749,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -788,7 +781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -824,7 +817,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -859,7 +852,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -891,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -926,7 +919,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -961,7 +954,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -993,7 +986,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1028,7 +1021,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1056,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>83</v>
       </c>
@@ -1098,7 +1091,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>89</v>
       </c>
@@ -1133,7 +1126,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
@@ -1165,7 +1158,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
@@ -1197,7 +1190,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
@@ -1226,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1258,62 +1251,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>114</v>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>45306</v>
+        <v>45275</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F17" s="8">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>52</v>
       </c>
       <c r="J17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>88</v>
+        <v>3</v>
+      </c>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3">
-        <v>45275</v>
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F18" s="8">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>52</v>
@@ -1321,140 +1315,107 @@
       <c r="J18">
         <v>3</v>
       </c>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>55</v>
+      <c r="D19" s="3">
+        <v>45261</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="F19" s="8">
         <v>100</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="J19">
         <v>3</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>112</v>
+        <v>29</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
       </c>
       <c r="D20" s="3">
         <v>45261</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F20" s="8">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="4">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3">
-        <v>45261</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="8">
-        <v>105</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+    <row r="21" spans="1:11" ht="43.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B21" s="10">
         <f>SUM(F:F)</f>
-        <v>1695</v>
-      </c>
+        <v>1610</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <f>_xlfn.QUARTILE.INC(C:C,1)</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24">
-        <f>_xlfn.QUARTILE.INC(C:C,1)</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <f>_xlfn.QUARTILE.INC(C:C,2)</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25">
-        <f>_xlfn.QUARTILE.INC(C:C,2)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <f>_xlfn.QUARTILE.INC(C:C,3)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26">
-        <f>_xlfn.QUARTILE.INC(C:C,3)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27">
         <f>_xlfn.QUARTILE.INC(C:C,4)</f>
         <v>61</v>
       </c>
@@ -1468,8 +1429,8 @@
     <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B4" r:id="rId10" xr:uid="{5F417FAE-548E-43C2-A72F-EFF6AAC0C847}"/>
     <hyperlink ref="B10" r:id="rId11" xr:uid="{CEBD452E-F47C-5C4A-B5D1-2D489AFAD36E}"/>
     <hyperlink ref="B11" r:id="rId12" xr:uid="{CE1B6F0B-99DB-644D-A9E8-6D3D507E9BD1}"/>
@@ -1478,12 +1439,11 @@
     <hyperlink ref="B14" r:id="rId15" xr:uid="{7C6CE824-AE30-494D-B258-0054A0D899EA}"/>
     <hyperlink ref="B15" r:id="rId16" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
     <hyperlink ref="B16" r:id="rId17" xr:uid="{1B93CA37-878D-49EE-B5EB-04AB17E9D9F3}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
-    <hyperlink ref="B17" r:id="rId20" xr:uid="{27EAEAD3-5A22-45D5-8B9B-93351924D911}"/>
+    <hyperlink ref="B17" r:id="rId18" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri"&amp;11&amp;K000000PERSONAL/NONWORK // EXTERNAL&amp;1#</oddHeader>
   </headerFooter>
@@ -1498,15 +1458,15 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.4609375" customWidth="1"/>
-    <col min="3" max="3" width="11.15234375" customWidth="1"/>
-    <col min="4" max="5" width="19.4609375" customWidth="1"/>
-    <col min="6" max="6" width="16.4609375" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="5" width="19.46484375" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1552,7 +1512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +1523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1582,7 +1542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1590,7 +1550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1558,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1606,7 +1566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1614,7 +1574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1622,7 +1582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1633,7 +1593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1641,7 +1601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1649,7 +1609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1660,7 +1620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1676,7 +1636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1684,7 +1644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1692,7 +1652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1700,7 +1660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1708,22 +1668,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1731,7 +1691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1739,7 +1699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1747,12 +1707,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Added a few schools
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\transit_credit-access\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E4F915-DA08-4200-8F1B-853A49E28E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2E7F4C-5E5C-CA4B-8441-30118D50ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30090" yWindow="2400" windowWidth="19830" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="131">
   <si>
     <t>School</t>
   </si>
@@ -261,12 +261,6 @@
     <t xml:space="preserve">Paul Ernesto Carrillo -- a few housing papers. Remi Jedwab -- cool urban development papers. Anthony Yezer -- real estate finance and urban development. </t>
   </si>
   <si>
-    <t>500 words</t>
-  </si>
-  <si>
-    <t>500 word diversity statement</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -345,12 +339,6 @@
     <t xml:space="preserve">Parag Pathak -- cool paper on CPS, race and school quality, etc. Nathaniel Hendren -- social mobility. Simon Jager -- labor. </t>
   </si>
   <si>
-    <t>They require a professional resume and an "analytical/quantitative resume", which is likely to overlap.</t>
-  </si>
-  <si>
-    <t>No SoP, but 6 essays. Ugh.</t>
-  </si>
-  <si>
     <t>Max 20 pages. IDK what that means.</t>
   </si>
   <si>
@@ -375,9 +363,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Same as PhD</t>
-  </si>
-  <si>
     <t>Distribution of Rankings</t>
   </si>
   <si>
@@ -421,6 +406,27 @@
   </si>
   <si>
     <t xml:space="preserve">The length of the writing sample might DQ this program for me. But I could use the Gary Becker discussion in my poli sci thesis </t>
+  </si>
+  <si>
+    <t>UVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Pepper -- cool policy evaluation work. Sarah Turner -- disparate returns to higher education, inequality. Amalia Miller -- gender labor papers. </t>
+  </si>
+  <si>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamein Cunningham (on leave at UT Austin) -- civil rights enforcement and racial wage gap, police brutality. Max Kapustin -- crime and urban econ. Douglas Miller -- housing fx on child mortality, EITC, head start. </t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>Min 200 words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Feigenbaum -- economic history. Martin Fiszbein -- demographics and political extremism. Adam Guren -- household finance and real estate. </t>
   </si>
 </sst>
 </file>
@@ -443,6 +449,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,18 +457,21 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -501,7 +511,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,6 +531,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -744,23 +756,23 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
@@ -795,7 +807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -803,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D2" s="5">
         <v>45204</v>
@@ -811,8 +823,8 @@
       <c r="E2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>113</v>
+      <c r="F2" s="11">
+        <v>0</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>51</v>
@@ -830,85 +842,88 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="D3" s="3">
         <v>45261</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="4">
+        <v>12</v>
       </c>
       <c r="D4" s="3">
         <v>45261</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="F4" s="8">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
+      <c r="K4" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
         <v>45261</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F5" s="8">
         <v>75</v>
@@ -920,53 +935,50 @@
         <v>55</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
         <v>45261</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F6" s="8">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>29</v>
@@ -975,230 +987,233 @@
         <v>4</v>
       </c>
       <c r="D7" s="3">
-        <v>45261</v>
+        <v>45264</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="F7" s="8">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
+      <c r="K7" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="D8" s="3">
-        <v>45264</v>
+        <v>45265</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="8">
-        <v>135</v>
+        <v>52</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45266</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6">
+        <v>95</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="3">
-        <v>45265</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45274</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="8">
+        <v>120</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45275</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="8">
+        <v>75</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="5">
-        <v>45266</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="6">
-        <v>200</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10">
+      <c r="J11">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="4">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3">
-        <v>45274</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="8">
-        <v>120</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>87</v>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="D12" s="3">
         <v>45275</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="F12" s="8">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J12">
         <v>3</v>
       </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="3">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="15">
         <v>45275</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="F13" s="8">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1230,7 +1245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1244,13 +1259,13 @@
         <v>45292</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F15" s="8">
         <v>75</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>55</v>
@@ -1262,10 +1277,10 @@
         <v>2</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1279,7 +1294,7 @@
         <v>45295</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" s="8">
         <v>90</v>
@@ -1288,7 +1303,7 @@
         <v>51</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>52</v>
@@ -1297,263 +1312,281 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="4">
-        <v>61</v>
-      </c>
-      <c r="D17" s="3">
-        <v>45306</v>
+        <v>8</v>
+      </c>
+      <c r="D17" s="15">
+        <v>45295</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="F17" s="8">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
+        <v>115</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>69</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>29</v>
+      </c>
+      <c r="C18" s="4">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45306</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="14">
-        <v>100</v>
+        <v>74</v>
+      </c>
+      <c r="F18" s="8">
+        <v>80</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
-        <v>91</v>
+      <c r="H18" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>52</v>
       </c>
       <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45306</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="8">
+        <v>85</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19">
         <v>2</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="15" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F20" s="14">
         <v>100</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="4">
-        <v>4</v>
-      </c>
-      <c r="D20" s="15">
-        <v>45275</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F20" s="8">
-        <v>75</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>14</v>
+      </c>
+      <c r="D21" s="15">
+        <v>45306</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="J20">
+      <c r="F21" s="8">
+        <v>105</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="4">
-        <v>8</v>
-      </c>
-      <c r="D21" s="15">
-        <v>45295</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="B22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4">
+        <v>22</v>
+      </c>
+      <c r="D22" s="15">
+        <v>45275</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="8">
         <v>95</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G22" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="H23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22">
+      <c r="J23">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="12"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="10">
         <f>SUM(F:F)</f>
-        <v>1780</v>
+        <v>1770</v>
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B26">
         <f>_xlfn.QUARTILE.INC(C:C,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B27">
         <f>_xlfn.QUARTILE.INC(C:C,2)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B28">
         <f>_xlfn.QUARTILE.INC(C:C,3)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B29">
         <f>_xlfn.QUARTILE.INC(C:C,4)</f>
@@ -1561,33 +1594,34 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
-    <sortCondition ref="D2:D31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K23">
+    <sortCondition ref="D3:D23"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{5F417FAE-548E-43C2-A72F-EFF6AAC0C847}"/>
-    <hyperlink ref="B5" r:id="rId11" xr:uid="{CEBD452E-F47C-5C4A-B5D1-2D489AFAD36E}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{CE1B6F0B-99DB-644D-A9E8-6D3D507E9BD1}"/>
-    <hyperlink ref="B6" r:id="rId13" xr:uid="{A4DEDE0E-6619-DB4E-9E11-376ABE075990}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{FF01F1E2-5FB2-F04F-9617-5DDCDCBF3B40}"/>
-    <hyperlink ref="B9" r:id="rId15" xr:uid="{7C6CE824-AE30-494D-B258-0054A0D899EA}"/>
-    <hyperlink ref="B22" r:id="rId16" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
-    <hyperlink ref="B16" r:id="rId17" xr:uid="{1B93CA37-878D-49EE-B5EB-04AB17E9D9F3}"/>
-    <hyperlink ref="B12" r:id="rId18" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
-    <hyperlink ref="B7" r:id="rId19" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{16F5FAE6-3B8C-4DCA-9610-8744A32C2BEA}"/>
+    <hyperlink ref="B18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{5F417FAE-548E-43C2-A72F-EFF6AAC0C847}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{CEBD452E-F47C-5C4A-B5D1-2D489AFAD36E}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{CE1B6F0B-99DB-644D-A9E8-6D3D507E9BD1}"/>
+    <hyperlink ref="B5" r:id="rId11" xr:uid="{A4DEDE0E-6619-DB4E-9E11-376ABE075990}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{FF01F1E2-5FB2-F04F-9617-5DDCDCBF3B40}"/>
+    <hyperlink ref="B8" r:id="rId13" xr:uid="{7C6CE824-AE30-494D-B258-0054A0D899EA}"/>
+    <hyperlink ref="B23" r:id="rId14" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{1B93CA37-878D-49EE-B5EB-04AB17E9D9F3}"/>
+    <hyperlink ref="B11" r:id="rId16" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
+    <hyperlink ref="B6" r:id="rId17" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
+    <hyperlink ref="B17" r:id="rId18" xr:uid="{16F5FAE6-3B8C-4DCA-9610-8744A32C2BEA}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{99892D0C-0151-D548-B7A6-3C28B40FD72B}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{18F082EC-0CC4-474C-BF73-7150C2252576}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{3FB740C0-1F81-874F-9865-53971F86B691}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri"&amp;11&amp;K000000PERSONAL/NONWORK // EXTERNAL&amp;1#</oddHeader>
   </headerFooter>
@@ -1602,15 +1636,15 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1656,7 +1690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1667,7 +1701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1678,7 +1712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1694,7 +1728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1702,7 +1736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1710,7 +1744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1718,7 +1752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1726,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1737,7 +1771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1745,7 +1779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1753,7 +1787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1764,7 +1798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1772,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1780,7 +1814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1788,7 +1822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1796,7 +1830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1804,7 +1838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1812,22 +1846,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1835,7 +1869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1843,7 +1877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1851,12 +1885,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
New versions of the SoP
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2E7F4C-5E5C-CA4B-8441-30118D50ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F185E11-0E11-9341-9142-56F48B7EF75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
   <si>
     <t>School</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t xml:space="preserve">James Feigenbaum -- economic history. Martin Fiszbein -- demographics and political extremism. Adam Guren -- household finance and real estate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthew Turner -- cool urbanization/infrastructure papers, incl subway papers. Lorenzo Lagos -- inequality and wage disparity. Jesse Bruhn -- public housing, education. </t>
   </si>
 </sst>
 </file>
@@ -753,11 +759,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1421,8 +1427,8 @@
       <c r="B20" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>55</v>
+      <c r="D20" s="3">
+        <v>45306</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>52</v>
@@ -1512,90 +1518,123 @@
       </c>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4">
+        <v>20</v>
+      </c>
+      <c r="D23" s="15">
+        <v>45292</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="8">
+        <v>75</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D24" s="15">
+        <v>45306</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="G24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23">
+      <c r="J24">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
+    <row r="25" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B25" s="10">
         <f>SUM(F:F)</f>
-        <v>1770</v>
-      </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26">
-        <f>_xlfn.QUARTILE.INC(C:C,1)</f>
-        <v>6</v>
-      </c>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27">
-        <f>_xlfn.QUARTILE.INC(C:C,2)</f>
-        <v>12</v>
+        <f>_xlfn.QUARTILE.INC(C:C,1)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28">
+        <f>_xlfn.QUARTILE.INC(C:C,2)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f>_xlfn.QUARTILE.INC(C:C,3)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <f>_xlfn.QUARTILE.INC(C:C,4)</f>
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K23">
-    <sortCondition ref="D3:D23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K24">
+    <sortCondition ref="D3:D24"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1611,7 +1650,7 @@
     <hyperlink ref="B5" r:id="rId11" xr:uid="{A4DEDE0E-6619-DB4E-9E11-376ABE075990}"/>
     <hyperlink ref="B20" r:id="rId12" xr:uid="{FF01F1E2-5FB2-F04F-9617-5DDCDCBF3B40}"/>
     <hyperlink ref="B8" r:id="rId13" xr:uid="{7C6CE824-AE30-494D-B258-0054A0D899EA}"/>
-    <hyperlink ref="B23" r:id="rId14" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{62B1ED50-7C87-9F42-94A8-5B286787503B}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{1B93CA37-878D-49EE-B5EB-04AB17E9D9F3}"/>
     <hyperlink ref="B11" r:id="rId16" xr:uid="{DE4CF150-431E-F943-B00A-9916FAE52C5A}"/>
     <hyperlink ref="B6" r:id="rId17" xr:uid="{758FF3B7-7422-4CA8-8353-6CEC896418A2}"/>
@@ -1619,9 +1658,10 @@
     <hyperlink ref="B19" r:id="rId19" xr:uid="{99892D0C-0151-D548-B7A6-3C28B40FD72B}"/>
     <hyperlink ref="B22" r:id="rId20" xr:uid="{18F082EC-0CC4-474C-BF73-7150C2252576}"/>
     <hyperlink ref="B21" r:id="rId21" xr:uid="{3FB740C0-1F81-874F-9865-53971F86B691}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{245EB07D-66D3-004B-9D45-1C5074223169}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri"&amp;11&amp;K000000PERSONAL/NONWORK // EXTERNAL&amp;1#</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Adding extenuating circumstances and a faculty member
</commit_message>
<xml_diff>
--- a/notes/Grad.schools.xlsx
+++ b/notes/Grad.schools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/transit_credit-access/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B7E533-418E-8848-8A5E-807F590EB36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84AD430-26DE-D94E-AD8F-A885CC7F633D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="500" windowWidth="19200" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application Details" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
     <t>Duke has a required 1-page diversity statement</t>
   </si>
   <si>
-    <t>Joseph Altonji -- cool research on the role of families and schools in inequality. Gerald Jaynes -- research on Black participation in the labor market and effects of migration on the Black work ytlacil -- evaluating disparate returns to schooling, speaks to disparate impact of treatment effects (like my NSF proposal).</t>
+    <t>Joseph Altonji -- cool research on the role of families and schools in inequality. Gerald Jaynes -- research on Black participation in the labor market and effects of migration on the Black work. Edward Vytlacil -- evaluating disparate returns to schooling, speaks to disparate impact of treatment effects (like my NSF proposal).</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>